<commit_message>
cap nhat xong 50% capstone
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/happynew/bài tập capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BC214B-E86A-774C-8F41-E6772D19E65F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CF957D-2F04-514D-9EED-93E0AA55966A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="32020" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -796,7 +796,7 @@
   <dimension ref="A1:J991"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.15"/>
@@ -1019,7 +1019,7 @@
         <v>44800</v>
       </c>
       <c r="D8" s="29">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="E8" s="26" t="s">
         <v>32</v>
@@ -1063,7 +1063,7 @@
         <v>44802</v>
       </c>
       <c r="D10" s="8">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E10" s="26" t="s">
         <v>32</v>
@@ -1084,7 +1084,9 @@
       <c r="C11" s="10">
         <v>44802</v>
       </c>
-      <c r="D11" s="8"/>
+      <c r="D11" s="8">
+        <v>1</v>
+      </c>
       <c r="E11" s="26" t="s">
         <v>32</v>
       </c>
@@ -1104,7 +1106,9 @@
       <c r="C12" s="10">
         <v>44802</v>
       </c>
-      <c r="D12" s="8"/>
+      <c r="D12" s="8">
+        <v>1</v>
+      </c>
       <c r="E12" s="27" t="s">
         <v>32</v>
       </c>
@@ -1124,7 +1128,9 @@
       <c r="C13" s="7">
         <v>44803</v>
       </c>
-      <c r="D13" s="8"/>
+      <c r="D13" s="8">
+        <v>1</v>
+      </c>
       <c r="E13" s="28" t="s">
         <v>32</v>
       </c>

</xml_diff>